<commit_message>
ndimas add more orders
</commit_message>
<xml_diff>
--- a/assets/data/merchant.xlsx
+++ b/assets/data/merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew2\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D13B879-8132-4C14-88BF-9257FC1E2A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD09B9E-821A-449C-93BC-7ABCD144D47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pandau Hilir, Kota Medan, Sumatera Utara, Sumatera, 20236, Indonesia</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>sebelah kertanadi food</t>
+  </si>
+  <si>
+    <t>Petisah, Kota Medan, Sumatera Utara, Sumatera, 20256, Indonesia</t>
+  </si>
+  <si>
+    <t>Sukabumi II, Kota Medan, Sumatera Utara, Sumatera, 20222, Indonesia</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,7 +422,7 @@
         <v>97.662300000000002</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -462,7 +468,7 @@
         <v>99.590500000000006</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ndimas orders fix done
</commit_message>
<xml_diff>
--- a/assets/data/merchant.xlsx
+++ b/assets/data/merchant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew2\flutter_application_1\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riand\Documents\tmp\flutter_app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F47C8F3-1F80-4C75-A89C-D4A0B3B78497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0B15A-A364-4AEC-8426-C6BE502297F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,20 +389,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -425,7 +425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>